<commit_message>
Added comments for read excel file
</commit_message>
<xml_diff>
--- a/Sheets.xlsx
+++ b/Sheets.xlsx
@@ -24,7 +24,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>A0.01</t>
+  </si>
+  <si>
+    <t>COVER SHEET</t>
+  </si>
+  <si>
+    <t>A2.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,17 +353,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>